<commit_message>
change excel file add ( and )
</commit_message>
<xml_diff>
--- a/Задание.xlsx
+++ b/Задание.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\labs-informatics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7811A8-5319-45DC-9E34-21EB71693B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF0F70C-4329-4209-9821-73E0E6A2CCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B555292D-57F1-4C62-ACDF-41778E11C24D}"/>
+    <workbookView xWindow="-225" yWindow="825" windowWidth="10890" windowHeight="9660" xr2:uid="{B555292D-57F1-4C62-ACDF-41778E11C24D}"/>
   </bookViews>
   <sheets>
     <sheet name="Задание 1-1" sheetId="1" r:id="rId1"/>
@@ -404,10 +404,13 @@
   <dimension ref="B3:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="57.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -420,8 +423,8 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <f>C4*C5*C3*C3 - (C5/SIN(C3/C5)*SIN(C3/C5))</f>
-        <v>1287.04</v>
+        <f>C4*C5*C3*C3 - (C5/(SIN(C3/C5)*SIN(C3/C5)))</f>
+        <v>1287.0239074715441</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix ambiguous naming for function && check triangle && fix formula for triangle
</commit_message>
<xml_diff>
--- a/Задание.xlsx
+++ b/Задание.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\labs-informatics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D983532-6419-4577-896B-226752232AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353CBAB9-528E-4B41-8AE2-B3431644C9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15705" yWindow="2085" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{B555292D-57F1-4C62-ACDF-41778E11C24D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B555292D-57F1-4C62-ACDF-41778E11C24D}"/>
   </bookViews>
   <sheets>
     <sheet name="Задание 1-1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Первая сторона</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Площадь треугольника</t>
+  </si>
+  <si>
+    <t>Полупериметр треугольника</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329AE516-0DAF-4D46-B514-EF88AC5B901D}">
-  <dimension ref="C4:I8"/>
+  <dimension ref="C4:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,8 +459,8 @@
         <v>4</v>
       </c>
       <c r="I7">
-        <f>SQRT((D4+D6+D8)*((D4+D6+D8)-D4)*((D4+D6+D8)-D6)*((D4+D6+D8)-D8))</f>
-        <v>44.090815370097204</v>
+        <f>SQRT(I11*(I11-D4)*(I11-D6)*(I11-D8))</f>
+        <v>3.897114317029974</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -466,6 +469,15 @@
       </c>
       <c r="D8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f>(D4+D6+D8)/2</f>
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>